<commit_message>
Added R0 and notes Markdown
Added R0 for datacleanup seperate from analyses, and my own Markdown for my own notes.
</commit_message>
<xml_diff>
--- a/data/desc_stats1.xlsx
+++ b/data/desc_stats1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ale\Desktop\USAtapData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u6047585\Documents\GitHub\CityWater\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3904061-40DF-451E-8420-70586F238202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Urban_Areas" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UA_time_slices!$A$1:$AO$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Urban_Areas!$A$1:$AI$24</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="293">
   <si>
     <t>Cluster_Location_Time</t>
   </si>
@@ -895,16 +896,25 @@
   </si>
   <si>
     <t>0500000US55063</t>
+  </si>
+  <si>
+    <t>Annual Rainfall</t>
+  </si>
+  <si>
+    <t>Streamflow within city</t>
+  </si>
+  <si>
+    <t>Topographic relief</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -924,8 +934,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -950,6 +967,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -960,10 +982,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -992,8 +1015,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1287,18 +1312,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="15"/>
-    <col min="2" max="3" width="13.42578125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="12" customWidth="1"/>
     <col min="4" max="14" width="11.42578125" style="15"/>
     <col min="15" max="15" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
@@ -4175,21 +4201,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ24"/>
+  <autoFilter ref="A1:AJ24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN29"/>
   <sheetViews>
     <sheetView topLeftCell="AF1" workbookViewId="0">
       <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22.5703125" customWidth="1"/>
@@ -7385,20 +7411,20 @@
       <c r="R29" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO26"/>
+  <autoFilter ref="A1:AO26" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="9"/>
@@ -7413,7 +7439,7 @@
     <col min="16" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>169</v>
       </c>
@@ -7435,16 +7461,16 @@
       <c r="G1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="24" t="s">
         <v>179</v>
       </c>
       <c r="L1" s="9" t="s">
@@ -7453,7 +7479,7 @@
       <c r="M1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="24" t="s">
         <v>182</v>
       </c>
       <c r="O1" s="9" t="s">
@@ -7465,8 +7491,17 @@
       <c r="Q1" s="9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>4</v>
       </c>
@@ -7522,7 +7557,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>4</v>
       </c>
@@ -7578,7 +7613,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>4</v>
       </c>
@@ -7634,7 +7669,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>6</v>
       </c>
@@ -7690,7 +7725,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>6</v>
       </c>
@@ -7746,7 +7781,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -7802,7 +7837,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -7858,7 +7893,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -7914,7 +7949,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -7970,7 +8005,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -8026,7 +8061,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -8082,7 +8117,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>6</v>
       </c>
@@ -8138,7 +8173,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>6</v>
       </c>
@@ -8194,7 +8229,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>6</v>
       </c>
@@ -8250,7 +8285,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>8</v>
       </c>

</xml_diff>